<commit_message>
Added columns to data model
</commit_message>
<xml_diff>
--- a/static_new/suspectDB.xlsx
+++ b/static_new/suspectDB.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AAAAAAAA\Desktop\Q\FFFFFFFF\cs373\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AAAAAAAA\Desktop\Q\FFFFFFFF\cs373\IDB\static_new\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,6 +15,7 @@
     <sheet name="Suspect" sheetId="1" r:id="rId1"/>
     <sheet name="State" sheetId="2" r:id="rId2"/>
     <sheet name="Crime" sheetId="3" r:id="rId3"/>
+    <sheet name="CrimeByState" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="191">
   <si>
     <t>Name</t>
   </si>
@@ -82,9 +83,6 @@
     <t>Kuwait</t>
   </si>
   <si>
-    <t>Country</t>
-  </si>
-  <si>
     <t>United States</t>
   </si>
   <si>
@@ -571,16 +569,37 @@
     <t>Arson</t>
   </si>
   <si>
-    <t>Kindapping</t>
-  </si>
-  <si>
-    <t>Child Pornography</t>
-  </si>
-  <si>
     <t>fk_CrimeID</t>
   </si>
   <si>
     <t>fk_StateID</t>
+  </si>
+  <si>
+    <t>Pornography/Obscene Material</t>
+  </si>
+  <si>
+    <t>Kindapping/Abduction</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Victims</t>
+  </si>
+  <si>
+    <t>Offenders</t>
+  </si>
+  <si>
+    <t>HomeCountry</t>
+  </si>
+  <si>
+    <t>EscapeCountry</t>
+  </si>
+  <si>
+    <t>Syria</t>
+  </si>
+  <si>
+    <t>Oman</t>
   </si>
 </sst>
 </file>
@@ -588,7 +607,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy/mm/dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -621,7 +640,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -902,22 +921,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" style="1" customWidth="1"/>
-    <col min="6" max="8" width="12.7109375" customWidth="1"/>
-    <col min="9" max="11" width="16.7109375" customWidth="1"/>
-    <col min="12" max="13" width="12.7109375" customWidth="1"/>
+    <col min="7" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="12" width="16.7109375" customWidth="1"/>
+    <col min="13" max="14" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -931,34 +950,37 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>187</v>
       </c>
       <c r="F1" t="s">
+        <v>188</v>
+      </c>
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
-        <v>183</v>
-      </c>
       <c r="M1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+      <c r="N1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -972,34 +994,37 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F2" t="s">
+        <v>189</v>
+      </c>
+      <c r="G2" t="s">
         <v>11</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>75</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>150</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>13</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>14</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>15</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>1</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1013,68 +1038,71 @@
         <v>17</v>
       </c>
       <c r="F3" t="s">
+        <v>190</v>
+      </c>
+      <c r="G3" t="s">
         <v>11</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>70</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>200</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>13</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>14</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>15</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>2</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1">
         <v>27977</v>
       </c>
       <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4">
+        <v>72</v>
+      </c>
+      <c r="I4">
+        <v>230</v>
+      </c>
+      <c r="J4" t="s">
         <v>22</v>
       </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4">
-        <v>72</v>
-      </c>
-      <c r="H4">
-        <v>230</v>
-      </c>
-      <c r="I4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>14</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>15</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>3</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>20</v>
       </c>
     </row>
@@ -1088,7 +1116,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
@@ -1099,16 +1127,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1116,13 +1144,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1130,13 +1158,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1144,13 +1172,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1158,13 +1186,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1172,13 +1200,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1186,13 +1214,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1200,13 +1228,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1214,13 +1242,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1228,13 +1256,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1242,13 +1270,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1256,13 +1284,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1270,13 +1298,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1284,13 +1312,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1298,13 +1326,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1312,13 +1340,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1326,13 +1354,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1340,13 +1368,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D18" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1354,13 +1382,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1368,13 +1396,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1382,13 +1410,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1396,13 +1424,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D22" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1410,13 +1438,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D23" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1424,13 +1452,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D24" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1438,13 +1466,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C25" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1452,13 +1480,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D26" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1466,13 +1494,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D27" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1480,13 +1508,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D28" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1494,13 +1522,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C29" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1508,13 +1536,13 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C30" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D30" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1522,13 +1550,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C31" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D31" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1536,13 +1564,13 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C32" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D32" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1550,13 +1578,13 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C33" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D33" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1564,13 +1592,13 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C34" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D34" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1578,13 +1606,13 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C35" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D35" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1592,13 +1620,13 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C36" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D36" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1606,13 +1634,13 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C37" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D37" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1620,13 +1648,13 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C38" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D38" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1634,13 +1662,13 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C39" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D39" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1648,13 +1676,13 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C40" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D40" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1662,13 +1690,13 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C41" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D41" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1676,13 +1704,13 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C42" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D42" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1690,13 +1718,13 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C43" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D43" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1704,13 +1732,13 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C44" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D44" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1718,13 +1746,13 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C45" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D45" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1732,13 +1760,13 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C46" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D46" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1746,13 +1774,13 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C47" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D47" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1760,13 +1788,13 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C48" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D48" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1774,10 +1802,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C49" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1785,13 +1813,13 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C50" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D50" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1799,13 +1827,13 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C51" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D51" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1813,13 +1841,13 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C52" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D52" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -1829,48 +1857,243 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" customWidth="1"/>
+    <col min="3" max="4" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+      <c r="C2">
+        <v>13917</v>
+      </c>
+      <c r="D2">
+        <v>13906</v>
+      </c>
+      <c r="E2">
+        <v>14993</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+      <c r="C3">
+        <v>16636</v>
+      </c>
+      <c r="D3">
+        <v>6402</v>
+      </c>
+      <c r="E3">
+        <v>6414</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>182</v>
+      </c>
+      <c r="C4">
+        <v>11013</v>
+      </c>
+      <c r="D4">
+        <v>13508</v>
+      </c>
+      <c r="E4">
+        <v>12092</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>35</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1281</v>
+      </c>
+      <c r="D5">
+        <v>1263</v>
+      </c>
+      <c r="E5">
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>35</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>1851</v>
+      </c>
+      <c r="D6">
+        <v>646</v>
+      </c>
+      <c r="E6">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>35</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>1042</v>
+      </c>
+      <c r="D7">
+        <v>1456</v>
+      </c>
+      <c r="E7">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>37</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>840</v>
+      </c>
+      <c r="D8">
+        <v>761</v>
+      </c>
+      <c r="E8">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>37</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>322</v>
+      </c>
+      <c r="D9">
+        <v>176</v>
+      </c>
+      <c r="E9">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>37</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>183</v>
+      </c>
+      <c r="D10">
+        <v>202</v>
+      </c>
+      <c r="E10">
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added State pop. attribute, WantedIn, WantedFor relations
</commit_message>
<xml_diff>
--- a/static_new/suspectDB.xlsx
+++ b/static_new/suspectDB.xlsx
@@ -15,7 +15,9 @@
     <sheet name="Suspect" sheetId="1" r:id="rId1"/>
     <sheet name="State" sheetId="2" r:id="rId2"/>
     <sheet name="Crime" sheetId="3" r:id="rId3"/>
-    <sheet name="CrimeByState" sheetId="4" r:id="rId4"/>
+    <sheet name="WantedIn" sheetId="5" r:id="rId4"/>
+    <sheet name="WantedFor" sheetId="6" r:id="rId5"/>
+    <sheet name="CrimeByState" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="193">
   <si>
     <t>Name</t>
   </si>
@@ -600,6 +602,12 @@
   </si>
   <si>
     <t>Oman</t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>fk_SuspectID</t>
   </si>
 </sst>
 </file>
@@ -921,11 +929,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -936,7 +942,7 @@
     <col min="13" max="14" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -973,14 +979,8 @@
       <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" t="s">
-        <v>180</v>
-      </c>
-      <c r="N1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1017,14 +1017,8 @@
       <c r="L2" t="s">
         <v>15</v>
       </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="N2">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1058,14 +1052,8 @@
       <c r="L3" t="s">
         <v>15</v>
       </c>
-      <c r="M3">
-        <v>2</v>
-      </c>
-      <c r="N3">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1098,12 +1086,6 @@
       </c>
       <c r="L4" t="s">
         <v>15</v>
-      </c>
-      <c r="M4">
-        <v>3</v>
-      </c>
-      <c r="N4">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1114,18 +1096,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -1138,8 +1118,11 @@
       <c r="D1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1152,8 +1135,11 @@
       <c r="D2" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>4863300</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1166,8 +1152,11 @@
       <c r="D3" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>741894</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1180,8 +1169,11 @@
       <c r="D4" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>6931071</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1194,8 +1186,11 @@
       <c r="D5" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>2988248</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1208,8 +1203,11 @@
       <c r="D6" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>39250017</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1222,8 +1220,11 @@
       <c r="D7" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>5540545</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1236,8 +1237,11 @@
       <c r="D8" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>3576452</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1250,8 +1254,11 @@
       <c r="D9" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>952065</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1264,8 +1271,11 @@
       <c r="D10" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>20612439</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1278,8 +1288,11 @@
       <c r="D11" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>10310371</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1292,8 +1305,11 @@
       <c r="D12" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>1428557</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1306,8 +1322,11 @@
       <c r="D13" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>1683140</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1320,8 +1339,11 @@
       <c r="D14" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>12801539</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1334,8 +1356,11 @@
       <c r="D15" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>6633053</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1348,8 +1373,11 @@
       <c r="D16" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>3134693</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1362,8 +1390,11 @@
       <c r="D17" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>2907289</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1376,8 +1407,11 @@
       <c r="D18" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>4436974</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1390,8 +1424,11 @@
       <c r="D19" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>4681666</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1404,8 +1441,11 @@
       <c r="D20" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>1331479</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1418,8 +1458,11 @@
       <c r="D21" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>6016447</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1432,8 +1475,11 @@
       <c r="D22" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>6811779</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1446,8 +1492,11 @@
       <c r="D23" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <v>9928300</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1460,8 +1509,11 @@
       <c r="D24" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <v>5519952</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1474,8 +1526,11 @@
       <c r="D25" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <v>2988726</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1488,8 +1543,11 @@
       <c r="D26" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <v>6093000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1502,8 +1560,11 @@
       <c r="D27" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <v>1042520</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1516,8 +1577,11 @@
       <c r="D28" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <v>1907116</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1530,8 +1594,11 @@
       <c r="D29" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <v>2940058</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1544,8 +1611,11 @@
       <c r="D30" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <v>1334795</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1558,8 +1628,11 @@
       <c r="D31" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <v>8944469</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1572,8 +1645,11 @@
       <c r="D32" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <v>2081015</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1586,8 +1662,11 @@
       <c r="D33" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <v>19745289</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1600,8 +1679,11 @@
       <c r="D34" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <v>10146788</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1614,8 +1696,11 @@
       <c r="D35" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <v>757952</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1628,8 +1713,11 @@
       <c r="D36" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <v>11614373</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1642,8 +1730,11 @@
       <c r="D37" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <v>3923561</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1656,8 +1747,11 @@
       <c r="D38" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <v>4093465</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1670,8 +1764,11 @@
       <c r="D39" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39">
+        <v>12784227</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1684,8 +1781,11 @@
       <c r="D40" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40">
+        <v>1056426</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1698,8 +1798,11 @@
       <c r="D41" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41">
+        <v>4961119</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1712,8 +1815,11 @@
       <c r="D42" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42">
+        <v>865454</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1726,8 +1832,11 @@
       <c r="D43" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43">
+        <v>6651194</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1740,8 +1849,11 @@
       <c r="D44" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44">
+        <v>27862596</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1754,8 +1866,11 @@
       <c r="D45" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45">
+        <v>3051217</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1768,8 +1883,11 @@
       <c r="D46" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46">
+        <v>624594</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1782,8 +1900,11 @@
       <c r="D47" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47">
+        <v>8411808</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1796,8 +1917,11 @@
       <c r="D48" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48">
+        <v>7288000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1807,8 +1931,11 @@
       <c r="C49" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49">
+        <v>681170</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1821,8 +1948,11 @@
       <c r="D50" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50">
+        <v>1831102</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1835,8 +1965,11 @@
       <c r="D51" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51">
+        <v>5778708</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1848,6 +1981,9 @@
       </c>
       <c r="D52" t="s">
         <v>177</v>
+      </c>
+      <c r="E52">
+        <v>585501</v>
       </c>
     </row>
   </sheetData>
@@ -1859,9 +1995,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1945,11 +2079,131 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>